<commit_message>
Fixed error with "Out of Work Benefits" label
</commit_message>
<xml_diff>
--- a/Final CPP Data.xlsx
+++ b/Final CPP Data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://impservihub.sharepoint.com/sites/tpi-benchmarking/Shared Documents/CPP Benchmarking/DATA LIBRARY/Shiny App/Data/To use in Shiny App/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\connachan.cara\Documents\CommunityPlanningOutcomesProfiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="377" documentId="19248E699512A27CF9BE08162F439C6A8DE0B79D" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{C2263FBA-3585-45B9-89FE-B6E313DC7580}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12060" windowHeight="615" firstSheet="15" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12060" windowHeight="615" firstSheet="15" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Front page - notes on data" sheetId="1" r:id="rId1"/>
@@ -262,51 +261,6 @@
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>Out Of Work Benefits_Raw data_2006/07</t>
-  </si>
-  <si>
-    <t>Out Of Work Benefits_Raw data_2007/08</t>
-  </si>
-  <si>
-    <t>Out Of Work Benefits_Raw data_2008/09</t>
-  </si>
-  <si>
-    <t>Out Of Work Benefits_Raw data_2009/10</t>
-  </si>
-  <si>
-    <t>Out Of Work Benefits_Raw data_2010/11</t>
-  </si>
-  <si>
-    <t>Out Of Work Benefits_Raw data_2011/12</t>
-  </si>
-  <si>
-    <t>Out Of Work Benefits_Raw data_2012/13</t>
-  </si>
-  <si>
-    <t>Out Of Work Benefits_Raw data_2013/14</t>
-  </si>
-  <si>
-    <t>Out Of Work Benefits_Raw data_2014/15</t>
-  </si>
-  <si>
-    <t>Out Of Work Benefits_Raw data_2015/16</t>
-  </si>
-  <si>
-    <t>Out Of Work Benefits_Raw data_2016/17</t>
-  </si>
-  <si>
-    <t>Out Of Work Benefits_Projected_2017/18</t>
-  </si>
-  <si>
-    <t>Out Of Work Benefits_Projected_2018/19</t>
-  </si>
-  <si>
-    <t>Out Of Work Benefits_Projected_2019/20</t>
-  </si>
-  <si>
-    <t>Out Of Work Benefits_Projected_2020/21</t>
   </si>
   <si>
     <t>Crime Rate_Raw data_2006/07</t>
@@ -826,6 +780,51 @@
   </si>
   <si>
     <t>Median Earnings_Raw data_2016/17</t>
+  </si>
+  <si>
+    <t>Out of Work Benefits_Raw data_2006/07</t>
+  </si>
+  <si>
+    <t>Out of Work Benefits_Raw data_2007/08</t>
+  </si>
+  <si>
+    <t>Out of Work Benefits_Raw data_2008/09</t>
+  </si>
+  <si>
+    <t>Out of Work Benefits_Raw data_2009/10</t>
+  </si>
+  <si>
+    <t>Out of Work Benefits_Raw data_2010/11</t>
+  </si>
+  <si>
+    <t>Out of Work Benefits_Raw data_2011/12</t>
+  </si>
+  <si>
+    <t>Out of Work Benefits_Raw data_2012/13</t>
+  </si>
+  <si>
+    <t>Out of Work Benefits_Raw data_2013/14</t>
+  </si>
+  <si>
+    <t>Out of Work Benefits_Raw data_2014/15</t>
+  </si>
+  <si>
+    <t>Out of Work Benefits_Raw data_2015/16</t>
+  </si>
+  <si>
+    <t>Out of Work Benefits_Raw data_2016/17</t>
+  </si>
+  <si>
+    <t>Out of Work Benefits_Projected_2017/18</t>
+  </si>
+  <si>
+    <t>Out of Work Benefits_Projected_2018/19</t>
+  </si>
+  <si>
+    <t>Out of Work Benefits_Projected_2019/20</t>
+  </si>
+  <si>
+    <t>Out of Work Benefits_Projected_2020/21</t>
   </si>
 </sst>
 </file>
@@ -1968,7 +1967,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="37" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1987,7 +1986,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2006,7 +2005,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -2042,7 +2041,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -2097,7 +2096,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2192,7 +2191,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2228,7 +2227,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2281,7 +2280,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -18605,10 +18604,10 @@
     <row r="1" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="8" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -18995,37 +18994,37 @@
     <row r="1" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
       <c r="B1" s="15" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="L1" s="15" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -20303,37 +20302,37 @@
     <row r="1" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="8" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -21611,49 +21610,49 @@
   <sheetData>
     <row r="1" spans="1:16" s="8" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -23327,49 +23326,49 @@
     <row r="1" spans="1:16" s="8" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="8" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -25043,37 +25042,37 @@
   <sheetData>
     <row r="1" spans="1:12" s="34" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="B1" s="41" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="H1" s="41" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="I1" s="41" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="J1" s="41" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="K1" s="41" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="L1" s="41" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -26339,8 +26338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26350,49 +26349,49 @@
   <sheetData>
     <row r="1" spans="1:17" s="8" customFormat="1" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
-        <v>73</v>
+        <v>246</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>74</v>
+        <v>247</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>75</v>
+        <v>248</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>76</v>
+        <v>249</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>77</v>
+        <v>250</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>78</v>
+        <v>251</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>79</v>
+        <v>252</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>80</v>
+        <v>253</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>81</v>
+        <v>254</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>82</v>
+        <v>255</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>83</v>
+        <v>256</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>84</v>
+        <v>257</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>85</v>
+        <v>258</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>86</v>
+        <v>259</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>87</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -28100,49 +28099,49 @@
   <sheetData>
     <row r="1" spans="1:16" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B1" s="41" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -29816,49 +29815,49 @@
     <row r="1" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="8" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="Q1" s="8"/>
     </row>
@@ -31521,7 +31520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -31534,49 +31533,49 @@
     <row r="1" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="30"/>
       <c r="B1" s="41" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="H1" s="41" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="I1" s="41" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="J1" s="41" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="K1" s="41" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="L1" s="41" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="M1" s="41" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="N1" s="41" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="O1" s="41" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="P1" s="41" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -33253,37 +33252,37 @@
         <v>33</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -34562,37 +34561,37 @@
     <row r="1" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A1" s="22"/>
       <c r="B1" s="8" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="H1" s="41" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="I1" s="41" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="J1" s="41" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="K1" s="41" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="L1" s="41" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -37216,37 +37215,37 @@
     <row r="1" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="13"/>
       <c r="B1" s="8" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="M1" s="14"/>
       <c r="N1" s="14"/>
@@ -38595,37 +38594,37 @@
         <v>33</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -42521,37 +42520,37 @@
     <row r="1" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
       <c r="B1" s="18" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="K1" s="18" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="L1" s="18" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -43814,6 +43813,29 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="4ea622ab-6d0b-4c8a-8736-27bd26b1fd54">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D8B37618F89864ABE738DE1DBF7EE19" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="970e8a530ac73319c376cd16fe2510cf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1543e12e-b41e-4b3f-8a83-41e12152c6a2" xmlns:ns3="4ea622ab-6d0b-4c8a-8736-27bd26b1fd54" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87390b8b6bdfe0a949635d3cf27d7a94" ns2:_="" ns3:_="">
     <xsd:import namespace="1543e12e-b41e-4b3f-8a83-41e12152c6a2"/>
@@ -44004,44 +44026,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="4ea622ab-6d0b-4c8a-8736-27bd26b1fd54">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53A62CF-6776-462A-8C9F-B15AB1E72883}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4724EAE4-ADED-4996-8793-973D115FDA12}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1543e12e-b41e-4b3f-8a83-41e12152c6a2"/>
-    <ds:schemaRef ds:uri="4ea622ab-6d0b-4c8a-8736-27bd26b1fd54"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -44064,9 +44052,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4724EAE4-ADED-4996-8793-973D115FDA12}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53A62CF-6776-462A-8C9F-B15AB1E72883}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1543e12e-b41e-4b3f-8a83-41e12152c6a2"/>
+    <ds:schemaRef ds:uri="4ea622ab-6d0b-4c8a-8736-27bd26b1fd54"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>